<commit_message>
anova for demog, food
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
+++ b/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\BMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB6BF46-7BEE-4D65-A4CF-D7D2E0462556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04185E26-8EC2-4966-868A-7F2ED0368A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23910" yWindow="-3030" windowWidth="22590" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25320" yWindow="-2670" windowWidth="22245" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="55">
   <si>
     <t>Plain means</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>Without Asians, n=3313,</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Education</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -337,27 +349,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1759,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U117" sqref="U117"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,6 +1777,8 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1814,15 +1825,15 @@
       <c r="B6" s="7">
         <v>27.719113573407199</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22">
+      <c r="E6" s="20"/>
+      <c r="F6" s="21">
         <f>B3-B6</f>
         <v>2.185995122245</v>
       </c>
-      <c r="G6" s="21"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="8" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1834,12 +1845,12 @@
       <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -1861,7 +1872,7 @@
       <c r="L11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="25" t="s">
         <v>23</v>
       </c>
       <c r="N11" s="1" t="s">
@@ -1881,7 +1892,7 @@
       <c r="E12">
         <v>1684.74063448117</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="22">
         <v>2.72429235933687E-303</v>
       </c>
       <c r="K12" t="str">
@@ -1897,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="16" t="str">
-        <f>IF(F12&lt;0.0001,"&lt;0.0001",IF(F12&lt;0.001,"&lt;0.001",IF(F12&lt;0.01,"&lt;0.01",ROUND(F12,3))))</f>
+        <f t="shared" ref="N12:N19" si="1">IF(F12&lt;0.0001,"&lt;0.0001",IF(F12&lt;0.001,"&lt;0.001",IF(F12&lt;0.01,"&lt;0.01",ROUND(F12,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S12" s="1" t="s">
@@ -1924,19 +1935,19 @@
         <v>5.7833871308588499E-3</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ref="K13:K19" si="1">B13</f>
+        <f t="shared" ref="K13:K19" si="2">B13</f>
         <v>DivGroup</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" ref="L13:L19" si="2">C13</f>
+        <f t="shared" ref="L13:L19" si="3">C13</f>
         <v>586.85806637862697</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M19" si="3">D13</f>
+        <f t="shared" ref="M13:M19" si="4">D13</f>
         <v>3</v>
       </c>
       <c r="N13" s="16" t="str">
-        <f>IF(F13&lt;0.0001,"&lt;0.0001",IF(F13&lt;0.001,"&lt;0.001",IF(F13&lt;0.01,"&lt;0.01",ROUND(F13,3))))</f>
+        <f t="shared" si="1"/>
         <v>&lt;0.01</v>
       </c>
       <c r="S13" t="s">
@@ -1964,26 +1975,26 @@
         <v>5.6693924408073503E-6</v>
       </c>
       <c r="K14" t="str">
+        <f t="shared" si="2"/>
+        <v>age_3</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="3"/>
+        <v>1133.9592419073199</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N14" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>age_3</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="2"/>
-        <v>1133.9592419073199</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="N14" s="16" t="str">
-        <f>IF(F14&lt;0.0001,"&lt;0.0001",IF(F14&lt;0.001,"&lt;0.001",IF(F14&lt;0.01,"&lt;0.01",ROUND(F14,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S14" t="s">
         <v>3</v>
       </c>
       <c r="T14" s="2">
-        <f t="shared" ref="T14:T16" si="4">C38</f>
+        <f t="shared" ref="T14:T16" si="5">C38</f>
         <v>29.268906677677698</v>
       </c>
     </row>
@@ -2004,26 +2015,26 @@
         <v>2.2784111178223801E-4</v>
       </c>
       <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v>RIAGENDR</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="3"/>
+        <v>636.82207392153202</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>RIAGENDR</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="2"/>
-        <v>636.82207392153202</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N15" s="16" t="str">
-        <f>IF(F15&lt;0.0001,"&lt;0.0001",IF(F15&lt;0.001,"&lt;0.001",IF(F15&lt;0.01,"&lt;0.01",ROUND(F15,3))))</f>
         <v>&lt;0.001</v>
       </c>
       <c r="S15" t="s">
         <v>4</v>
       </c>
       <c r="T15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.032998975001501</v>
       </c>
     </row>
@@ -2044,26 +2055,26 @@
         <v>1.16932824838311E-27</v>
       </c>
       <c r="K16" t="str">
+        <f t="shared" si="2"/>
+        <v>eth_5</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="3"/>
+        <v>6307.2496720910704</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N16" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>eth_5</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="2"/>
-        <v>6307.2496720910704</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="N16" s="16" t="str">
-        <f>IF(F16&lt;0.0001,"&lt;0.0001",IF(F16&lt;0.001,"&lt;0.001",IF(F16&lt;0.01,"&lt;0.01",ROUND(F16,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S16" t="s">
         <v>5</v>
       </c>
       <c r="T16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.861430808584899</v>
       </c>
     </row>
@@ -2084,52 +2095,52 @@
         <v>0.46186551847438101</v>
       </c>
       <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v>FIPL</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="3"/>
+        <v>72.287068934063399</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N17" s="16">
         <f t="shared" si="1"/>
-        <v>FIPL</v>
-      </c>
-      <c r="L17" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2">
+        <v>794.72141912972404</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>8.4944265337995404</v>
+      </c>
+      <c r="F18">
+        <v>2.0866660498913099E-4</v>
+      </c>
+      <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>72.287068934063399</v>
-      </c>
-      <c r="M17">
+        <v>edu</v>
+      </c>
+      <c r="L18" s="2">
         <f t="shared" si="3"/>
+        <v>794.72141912972404</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="N17" s="16">
-        <f>IF(F17&lt;0.0001,"&lt;0.0001",IF(F17&lt;0.001,"&lt;0.001",IF(F17&lt;0.01,"&lt;0.01",ROUND(F17,3))))</f>
-        <v>0.46200000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="25">
-        <v>794.72141912972404</v>
-      </c>
-      <c r="D18" s="24">
-        <v>2</v>
-      </c>
-      <c r="E18" s="24">
-        <v>8.4944265337995404</v>
-      </c>
-      <c r="F18" s="24">
-        <v>2.0866660498913099E-4</v>
-      </c>
-      <c r="K18" t="str">
+      <c r="N18" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>edu</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="2"/>
-        <v>794.72141912972404</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="N18" s="16" t="str">
-        <f>IF(F18&lt;0.0001,"&lt;0.0001",IF(F18&lt;0.001,"&lt;0.001",IF(F18&lt;0.01,"&lt;0.01",ROUND(F18,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -2150,19 +2161,19 @@
         <v>0.177245926697293</v>
       </c>
       <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v>KCAL</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="3"/>
+        <v>85.197064413921893</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="16">
         <f t="shared" si="1"/>
-        <v>KCAL</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="2"/>
-        <v>85.197064413921893</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N19" s="16">
-        <f>IF(F19&lt;0.0001,"&lt;0.0001",IF(F19&lt;0.001,"&lt;0.001",IF(F19&lt;0.01,"&lt;0.01",ROUND(F19,3))))</f>
         <v>0.17699999999999999</v>
       </c>
     </row>
@@ -2183,24 +2194,17 @@
         <v>27</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ref="K20" si="5">B20</f>
+        <f t="shared" ref="K20" si="6">B20</f>
         <v>Residuals</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" ref="L20" si="6">C20</f>
+        <f t="shared" ref="L20" si="7">C20</f>
         <v>171211.110158</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20" si="7">D20</f>
+        <f t="shared" ref="M20" si="8">D20</f>
         <v>3660</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2395,7 +2399,7 @@
       <c r="G28" s="4">
         <v>0.70675927343141898</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="23">
         <f>O28</f>
         <v>0.99928982412289802</v>
       </c>
@@ -2441,7 +2445,7 @@
       <c r="G29">
         <v>1.3434614109218299</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="24">
         <f>O29</f>
         <v>0.95923428424052004</v>
       </c>
@@ -2487,8 +2491,8 @@
       <c r="G30" s="8">
         <v>2.5208494114832001</v>
       </c>
-      <c r="H30" s="35">
-        <f t="shared" ref="H30:H33" si="8">O30</f>
+      <c r="H30" s="30">
+        <f t="shared" ref="H30:H33" si="9">O30</f>
         <v>4.2718020720824397E-3</v>
       </c>
       <c r="J30" t="s">
@@ -2533,8 +2537,8 @@
       <c r="G31">
         <v>1.4148485185347801</v>
       </c>
-      <c r="H31" s="27">
-        <f t="shared" si="8"/>
+      <c r="H31" s="24">
+        <f t="shared" si="9"/>
         <v>0.94326527426404705</v>
       </c>
       <c r="J31" t="s">
@@ -2579,8 +2583,8 @@
       <c r="G32" s="8">
         <v>2.58767858039805</v>
       </c>
-      <c r="H32" s="35">
-        <f t="shared" si="8"/>
+      <c r="H32" s="30">
+        <f t="shared" si="9"/>
         <v>4.5390494278589903E-3</v>
       </c>
       <c r="J32" t="s">
@@ -2625,8 +2629,8 @@
       <c r="G33" s="14">
         <v>2.6049217626543699</v>
       </c>
-      <c r="H33" s="34">
-        <f t="shared" si="8"/>
+      <c r="H33" s="29">
+        <f t="shared" si="9"/>
         <v>9.9163587106149406E-2</v>
       </c>
       <c r="J33" t="s">
@@ -2650,16 +2654,16 @@
       <c r="P33" s="13"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -2693,27 +2697,27 @@
         <v>DivNA</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" ref="B37:G37" si="9">B24</f>
+        <f t="shared" ref="B37:G37" si="10">B24</f>
         <v>.</v>
       </c>
       <c r="C37" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29.235780665700101</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.20744368005802699</v>
       </c>
       <c r="E37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3660</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>28.6531258747649</v>
       </c>
       <c r="G37" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29.8184354566352</v>
       </c>
       <c r="H37" t="s">
@@ -2722,31 +2726,31 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" ref="A38:G38" si="10">A25</f>
+        <f t="shared" ref="A38:G38" si="11">A25</f>
         <v>Div0</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>.</v>
       </c>
       <c r="C38" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>29.268906677677698</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.24229782292035801</v>
       </c>
       <c r="E38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3660</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>28.588355757455801</v>
       </c>
       <c r="G38" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>29.949457597899599</v>
       </c>
       <c r="H38" t="s">
@@ -2755,31 +2759,31 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" ref="A39:G39" si="11">A26</f>
+        <f t="shared" ref="A39:G39" si="12">A26</f>
         <v>Div1</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>.</v>
       </c>
       <c r="C39" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>29.032998975001501</v>
       </c>
       <c r="D39" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.38364715694239898</v>
       </c>
       <c r="E39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3660</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>27.955434915404101</v>
       </c>
       <c r="G39" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30.110563034598801</v>
       </c>
       <c r="H39" t="s">
@@ -2788,31 +2792,31 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" ref="A40:G40" si="12">A27</f>
+        <f t="shared" ref="A40:G40" si="13">A27</f>
         <v>Div2</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>.</v>
       </c>
       <c r="C40" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>27.861430808584899</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.38864921832963301</v>
       </c>
       <c r="E40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3660</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26.769817272855001</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>28.953044344314801</v>
       </c>
       <c r="H40" t="s">
@@ -2821,31 +2825,31 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f t="shared" ref="A41:G41" si="13">A28</f>
+        <f t="shared" ref="A41:G41" si="14">A28</f>
         <v>.</v>
       </c>
       <c r="B41" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>DivNA - Div0</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-3.31260119776439E-2</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.263422748450582</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3660</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.77301129738670704</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.70675927343141898</v>
       </c>
       <c r="H41" s="17">
@@ -2854,182 +2858,182 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="str">
-        <f t="shared" ref="A42:G42" si="14">A29</f>
+      <c r="A42" t="str">
+        <f t="shared" ref="A42:G42" si="15">A29</f>
         <v>.</v>
       </c>
-      <c r="B42" s="24" t="str">
-        <f t="shared" si="14"/>
+      <c r="B42" t="str">
+        <f t="shared" si="15"/>
         <v>DivNA - Div1</v>
       </c>
-      <c r="C42" s="30">
-        <f t="shared" si="14"/>
+      <c r="C42" s="6">
+        <f t="shared" si="15"/>
         <v>0.20278169069857699</v>
       </c>
-      <c r="D42" s="30">
-        <f t="shared" si="14"/>
+      <c r="D42" s="6">
+        <f t="shared" si="15"/>
         <v>0.40611834419294202</v>
       </c>
-      <c r="E42" s="24">
-        <f t="shared" si="14"/>
+      <c r="E42">
+        <f t="shared" si="15"/>
         <v>3660</v>
       </c>
-      <c r="F42" s="30">
-        <f t="shared" si="14"/>
+      <c r="F42" s="6">
+        <f t="shared" si="15"/>
         <v>-0.93789802952468004</v>
       </c>
-      <c r="G42" s="30">
-        <f t="shared" si="14"/>
+      <c r="G42" s="6">
+        <f t="shared" si="15"/>
         <v>1.3434614109218299</v>
       </c>
-      <c r="H42" s="29">
-        <f t="shared" ref="H42:H46" si="15">IF(H29&lt;0.0001,"&lt;0.0001",IF(H29&lt;0.001,"&lt;0.001",IF(H29&lt;0.01,"&lt;0.01",ROUND(H29,3))))</f>
+      <c r="H42" s="16">
+        <f t="shared" ref="H42:H46" si="16">IF(H29&lt;0.0001,"&lt;0.0001",IF(H29&lt;0.001,"&lt;0.001",IF(H29&lt;0.01,"&lt;0.01",ROUND(H29,3))))</f>
         <v>0.95899999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="str">
-        <f t="shared" ref="A43:G43" si="16">A30</f>
+      <c r="A43" t="str">
+        <f t="shared" ref="A43:G43" si="17">A30</f>
         <v>.</v>
       </c>
-      <c r="B43" s="24" t="str">
-        <f t="shared" si="16"/>
+      <c r="B43" t="str">
+        <f t="shared" si="17"/>
         <v>DivNA - Div2</v>
       </c>
-      <c r="C43" s="30">
-        <f t="shared" si="16"/>
+      <c r="C43" s="6">
+        <f t="shared" si="17"/>
         <v>1.37434985711516</v>
       </c>
-      <c r="D43" s="30">
-        <f t="shared" si="16"/>
+      <c r="D43" s="6">
+        <f t="shared" si="17"/>
         <v>0.40819039067930901</v>
       </c>
-      <c r="E43" s="24">
-        <f t="shared" si="16"/>
-        <v>3660</v>
-      </c>
-      <c r="F43" s="30">
-        <f t="shared" si="16"/>
-        <v>0.22785030274711399</v>
-      </c>
-      <c r="G43" s="30">
-        <f t="shared" si="16"/>
-        <v>2.5208494114832001</v>
-      </c>
-      <c r="H43" s="29" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;0.01</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="str">
-        <f t="shared" ref="A44:G44" si="17">A31</f>
-        <v>.</v>
-      </c>
-      <c r="B44" s="24" t="str">
-        <f t="shared" si="17"/>
-        <v>Div0 - Div1</v>
-      </c>
-      <c r="C44" s="30">
-        <f t="shared" si="17"/>
-        <v>0.23590770267622099</v>
-      </c>
-      <c r="D44" s="30">
-        <f t="shared" si="17"/>
-        <v>0.419740513966744</v>
-      </c>
-      <c r="E44" s="24">
+      <c r="E43">
         <f t="shared" si="17"/>
         <v>3660</v>
       </c>
-      <c r="F44" s="30">
+      <c r="F43" s="6">
         <f t="shared" si="17"/>
-        <v>-0.94303311318233296</v>
-      </c>
-      <c r="G44" s="30">
+        <v>0.22785030274711399</v>
+      </c>
+      <c r="G43" s="6">
         <f t="shared" si="17"/>
-        <v>1.4148485185347801</v>
-      </c>
-      <c r="H44" s="29">
-        <f t="shared" si="15"/>
-        <v>0.94299999999999995</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="str">
-        <f t="shared" ref="A45:G45" si="18">A32</f>
+        <v>2.5208494114832001</v>
+      </c>
+      <c r="H43" s="16" t="str">
+        <f t="shared" si="16"/>
+        <v>&lt;0.01</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f t="shared" ref="A44:G44" si="18">A31</f>
         <v>.</v>
       </c>
-      <c r="B45" s="24" t="str">
+      <c r="B44" t="str">
         <f t="shared" si="18"/>
-        <v>Div0 - Div2</v>
-      </c>
-      <c r="C45" s="30">
+        <v>Div0 - Div1</v>
+      </c>
+      <c r="C44" s="6">
         <f t="shared" si="18"/>
-        <v>1.4074758690928</v>
-      </c>
-      <c r="D45" s="30">
+        <v>0.23590770267622099</v>
+      </c>
+      <c r="D44" s="6">
         <f t="shared" si="18"/>
-        <v>0.42018978897380499</v>
-      </c>
-      <c r="E45" s="24">
+        <v>0.419740513966744</v>
+      </c>
+      <c r="E44">
         <f t="shared" si="18"/>
         <v>3660</v>
       </c>
-      <c r="F45" s="30">
+      <c r="F44" s="6">
         <f t="shared" si="18"/>
+        <v>-0.94303311318233296</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="18"/>
+        <v>1.4148485185347801</v>
+      </c>
+      <c r="H44" s="16">
+        <f t="shared" si="16"/>
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f t="shared" ref="A45:G45" si="19">A32</f>
+        <v>.</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="19"/>
+        <v>Div0 - Div2</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="19"/>
+        <v>1.4074758690928</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" si="19"/>
+        <v>0.42018978897380499</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="19"/>
+        <v>3660</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="19"/>
         <v>0.227273157787552</v>
       </c>
-      <c r="G45" s="30">
-        <f t="shared" si="18"/>
+      <c r="G45" s="6">
+        <f t="shared" si="19"/>
         <v>2.58767858039805</v>
       </c>
-      <c r="H45" s="29" t="str">
-        <f t="shared" si="15"/>
+      <c r="H45" s="16" t="str">
+        <f t="shared" si="16"/>
         <v>&lt;0.01</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
-        <f t="shared" ref="A46:G46" si="19">A33</f>
+        <f t="shared" ref="A46:G46" si="20">A33</f>
         <v>.</v>
       </c>
       <c r="B46" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Div1 - Div2</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.17156816641658</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.510319574221201</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3660</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-0.261785429821211</v>
       </c>
       <c r="G46" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.6049217626543699</v>
       </c>
       <c r="H46" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+    <row r="49" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="50" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3037,12 +3041,12 @@
       <c r="B51" t="s">
         <v>43</v>
       </c>
-      <c r="K51" s="31" t="s">
+      <c r="K51" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="27"/>
+      <c r="N51" s="27"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
@@ -3058,13 +3062,14 @@
         <v>24</v>
       </c>
       <c r="F52" s="1"/>
-      <c r="K52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="K52" s="1"/>
       <c r="L52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M52" s="28" t="s">
+      <c r="M52" s="25" t="s">
         <v>23</v>
       </c>
       <c r="N52" s="1" t="s">
@@ -3084,19 +3089,22 @@
       <c r="E53">
         <v>3473.75588051665</v>
       </c>
-      <c r="F53" s="23">
+      <c r="F53" s="22">
         <v>0</v>
       </c>
-      <c r="K53" t="str">
+      <c r="J53" t="str">
         <f>B53</f>
         <v>(Intercept)</v>
       </c>
+      <c r="K53" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="L53" s="2">
-        <f t="shared" ref="L53:L59" si="20">C53</f>
+        <f>C53</f>
         <v>162511.09889396001</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M59" si="21">D53</f>
+        <f>D53</f>
         <v>1</v>
       </c>
       <c r="N53" s="16" t="str">
@@ -3120,16 +3128,19 @@
       <c r="F54" s="10">
         <v>7.8334967627301504E-3</v>
       </c>
-      <c r="K54" t="str">
-        <f t="shared" ref="K54:K59" si="22">B54</f>
+      <c r="J54" t="str">
+        <f>B54</f>
         <v>DivGroup</v>
       </c>
+      <c r="K54" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="L54" s="2">
-        <f t="shared" si="20"/>
+        <f>C54</f>
         <v>556.24338689094304</v>
       </c>
       <c r="M54">
-        <f t="shared" si="21"/>
+        <f>D54</f>
         <v>3</v>
       </c>
       <c r="N54" s="16" t="str">
@@ -3153,16 +3164,19 @@
       <c r="F55" s="10">
         <v>9.3531943800360201E-6</v>
       </c>
-      <c r="K55" t="str">
-        <f t="shared" si="22"/>
+      <c r="J55" t="str">
+        <f>B55</f>
         <v>age_3</v>
       </c>
+      <c r="K55" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="L55" s="2">
-        <f t="shared" si="20"/>
+        <f>C55</f>
         <v>1086.89643039514</v>
       </c>
       <c r="M55">
-        <f t="shared" si="21"/>
+        <f>D55</f>
         <v>2</v>
       </c>
       <c r="N55" s="16" t="str">
@@ -3186,16 +3200,19 @@
       <c r="F56" s="10">
         <v>5.5744985372722195E-4</v>
       </c>
-      <c r="K56" t="str">
-        <f t="shared" si="22"/>
+      <c r="J56" t="str">
+        <f>B56</f>
         <v>RIAGENDR</v>
       </c>
+      <c r="K56" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="L56" s="2">
-        <f t="shared" si="20"/>
+        <f>C56</f>
         <v>558.30163286940694</v>
       </c>
       <c r="M56">
-        <f t="shared" si="21"/>
+        <f>D56</f>
         <v>1</v>
       </c>
       <c r="N56" s="16" t="str">
@@ -3219,16 +3236,19 @@
       <c r="F57" s="10">
         <v>7.5128152696058003E-29</v>
       </c>
-      <c r="K57" t="str">
-        <f t="shared" si="22"/>
+      <c r="J57" t="str">
+        <f>B57</f>
         <v>eth_5</v>
       </c>
+      <c r="K57" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="L57" s="2">
-        <f t="shared" si="20"/>
+        <f>C57</f>
         <v>6577.9944277828599</v>
       </c>
       <c r="M57">
-        <f t="shared" si="21"/>
+        <f>D57</f>
         <v>4</v>
       </c>
       <c r="N57" s="16" t="str">
@@ -3252,16 +3272,19 @@
       <c r="F58" s="10">
         <v>7.7620295626634899E-5</v>
       </c>
-      <c r="K58" t="str">
-        <f t="shared" si="22"/>
+      <c r="J58" t="str">
+        <f>B58</f>
         <v>edu</v>
       </c>
+      <c r="K58" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="L58" s="2">
-        <f t="shared" si="20"/>
+        <f>C58</f>
         <v>887.76162924518599</v>
       </c>
       <c r="M58">
-        <f t="shared" si="21"/>
+        <f>D58</f>
         <v>2</v>
       </c>
       <c r="N58" s="16" t="str">
@@ -3270,34 +3293,37 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="24" t="s">
+      <c r="B59" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="25">
+      <c r="C59" s="2">
         <v>171364.41814674699</v>
       </c>
-      <c r="D59" s="24">
+      <c r="D59">
         <v>3663</v>
       </c>
-      <c r="E59" s="24" t="s">
+      <c r="E59" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="24" t="s">
+      <c r="F59" t="s">
         <v>27</v>
       </c>
-      <c r="K59" t="str">
-        <f t="shared" si="22"/>
+      <c r="J59" t="str">
+        <f>B59</f>
         <v>Residuals</v>
       </c>
-      <c r="L59" s="2">
-        <f t="shared" si="20"/>
+      <c r="K59" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="32">
+        <f>C59</f>
         <v>171364.41814674699</v>
       </c>
-      <c r="M59">
-        <f t="shared" si="21"/>
+      <c r="M59" s="1">
+        <f>D59</f>
         <v>3663</v>
       </c>
-      <c r="N59" s="16"/>
+      <c r="N59" s="33"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C60" s="2"/>
@@ -3312,13 +3338,6 @@
       <c r="F61" s="1"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-    </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>44</v>
@@ -3512,7 +3531,7 @@
       <c r="G69" s="4">
         <v>0.68434796313179402</v>
       </c>
-      <c r="H69" s="26">
+      <c r="H69" s="23">
         <f>O69</f>
         <v>0.99705681946439695</v>
       </c>
@@ -3558,7 +3577,7 @@
       <c r="G70">
         <v>1.3145366893266699</v>
       </c>
-      <c r="H70" s="27">
+      <c r="H70" s="24">
         <f>O70</f>
         <v>0.97054718367815895</v>
       </c>
@@ -3604,8 +3623,8 @@
       <c r="G71" s="8">
         <v>2.4524342552881802</v>
       </c>
-      <c r="H71" s="35">
-        <f t="shared" ref="H71:H74" si="23">O71</f>
+      <c r="H71" s="30">
+        <f t="shared" ref="H71:H74" si="21">O71</f>
         <v>6.1601056166932198E-3</v>
       </c>
       <c r="J71" t="s">
@@ -3650,8 +3669,8 @@
       <c r="G72">
         <v>1.4103291709653401</v>
       </c>
-      <c r="H72" s="27">
-        <f t="shared" si="23"/>
+      <c r="H72" s="24">
+        <f t="shared" si="21"/>
         <v>0.944913683186826</v>
       </c>
       <c r="J72" t="s">
@@ -3696,8 +3715,8 @@
       <c r="G73" s="8">
         <v>2.5464065089600099</v>
       </c>
-      <c r="H73" s="35">
-        <f t="shared" si="23"/>
+      <c r="H73" s="30">
+        <f t="shared" si="21"/>
         <v>5.8718989702371003E-3</v>
       </c>
       <c r="J73" t="s">
@@ -3742,8 +3761,8 @@
       <c r="G74" s="14">
         <v>2.56948890902046</v>
       </c>
-      <c r="H74" s="34">
-        <f t="shared" si="23"/>
+      <c r="H74" s="29">
+        <f t="shared" si="21"/>
         <v>0.114845483404781</v>
       </c>
       <c r="J74" t="s">
@@ -3767,16 +3786,16 @@
       <c r="P74" s="13"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="32"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -3810,159 +3829,159 @@
         <v>DivNA</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" ref="B78:G78" si="24">B65</f>
+        <f t="shared" ref="B78:G78" si="22">B65</f>
         <v>.</v>
       </c>
       <c r="C78" s="6">
+        <f t="shared" si="22"/>
+        <v>29.261591650725599</v>
+      </c>
+      <c r="D78" s="6">
+        <f t="shared" si="22"/>
+        <v>0.202343551614832</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="22"/>
+        <v>3663</v>
+      </c>
+      <c r="F78" s="6">
+        <f t="shared" si="22"/>
+        <v>28.6932620629746</v>
+      </c>
+      <c r="G78" s="6">
+        <f t="shared" si="22"/>
+        <v>29.829921238476601</v>
+      </c>
+      <c r="H78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
+        <f t="shared" ref="A79:G79" si="23">A66</f>
+        <v>Div0</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="23"/>
+        <v>.</v>
+      </c>
+      <c r="C79" s="6">
+        <f t="shared" si="23"/>
+        <v>29.314800769417001</v>
+      </c>
+      <c r="D79" s="6">
+        <f t="shared" si="23"/>
+        <v>0.23879972063565899</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="23"/>
+        <v>3663</v>
+      </c>
+      <c r="F79" s="6">
+        <f t="shared" si="23"/>
+        <v>28.6440754327269</v>
+      </c>
+      <c r="G79" s="6">
+        <f t="shared" si="23"/>
+        <v>29.985526106107098</v>
+      </c>
+      <c r="H79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f t="shared" ref="A80:G80" si="24">A67</f>
+        <v>Div1</v>
+      </c>
+      <c r="B80" t="str">
         <f t="shared" si="24"/>
-        <v>29.261591650725599</v>
-      </c>
-      <c r="D78" s="6">
+        <v>.</v>
+      </c>
+      <c r="C80" s="6">
         <f t="shared" si="24"/>
-        <v>0.202343551614832</v>
-      </c>
-      <c r="E78">
+        <v>29.0817238483944</v>
+      </c>
+      <c r="D80" s="6">
+        <f t="shared" si="24"/>
+        <v>0.38212105318570799</v>
+      </c>
+      <c r="E80">
         <f t="shared" si="24"/>
         <v>3663</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F80" s="6">
         <f t="shared" si="24"/>
-        <v>28.6932620629746</v>
-      </c>
-      <c r="G78" s="6">
+        <v>28.0084467466788</v>
+      </c>
+      <c r="G80" s="6">
         <f t="shared" si="24"/>
-        <v>29.829921238476601</v>
-      </c>
-      <c r="H78" t="s">
+        <v>30.1550009501101</v>
+      </c>
+      <c r="H80" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A79" t="str">
-        <f t="shared" ref="A79:G79" si="25">A66</f>
-        <v>Div0</v>
-      </c>
-      <c r="B79" t="str">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f t="shared" ref="A81:G81" si="25">A68</f>
+        <v>Div2</v>
+      </c>
+      <c r="B81" t="str">
         <f t="shared" si="25"/>
         <v>.</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C81" s="6">
         <f t="shared" si="25"/>
-        <v>29.314800769417001</v>
-      </c>
-      <c r="D79" s="6">
+        <v>27.943991726981899</v>
+      </c>
+      <c r="D81" s="6">
         <f t="shared" si="25"/>
-        <v>0.23879972063565899</v>
-      </c>
-      <c r="E79">
+        <v>0.38424887385039203</v>
+      </c>
+      <c r="E81">
         <f t="shared" si="25"/>
         <v>3663</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F81" s="6">
         <f t="shared" si="25"/>
-        <v>28.6440754327269</v>
-      </c>
-      <c r="G79" s="6">
+        <v>26.864738139079702</v>
+      </c>
+      <c r="G81" s="6">
         <f t="shared" si="25"/>
-        <v>29.985526106107098</v>
-      </c>
-      <c r="H79" t="s">
+        <v>29.0232453148842</v>
+      </c>
+      <c r="H81" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80" t="str">
-        <f t="shared" ref="A80:G80" si="26">A67</f>
-        <v>Div1</v>
-      </c>
-      <c r="B80" t="str">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="str">
+        <f t="shared" ref="A82:G82" si="26">A69</f>
+        <v>.</v>
+      </c>
+      <c r="B82" s="4" t="str">
         <f t="shared" si="26"/>
-        <v>.</v>
-      </c>
-      <c r="C80" s="6">
+        <v>DivNA - Div0</v>
+      </c>
+      <c r="C82" s="5">
         <f t="shared" si="26"/>
-        <v>29.0817238483944</v>
-      </c>
-      <c r="D80" s="6">
+        <v>-5.3209118691406397E-2</v>
+      </c>
+      <c r="D82" s="5">
         <f t="shared" si="26"/>
-        <v>0.38212105318570799</v>
-      </c>
-      <c r="E80">
+        <v>0.26259396426173198</v>
+      </c>
+      <c r="E82" s="4">
         <f t="shared" si="26"/>
         <v>3663</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F82" s="5">
         <f t="shared" si="26"/>
-        <v>28.0084467466788</v>
-      </c>
-      <c r="G80" s="6">
+        <v>-0.790766200514607</v>
+      </c>
+      <c r="G82" s="5">
         <f t="shared" si="26"/>
-        <v>30.1550009501101</v>
-      </c>
-      <c r="H80" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" t="str">
-        <f t="shared" ref="A81:G81" si="27">A68</f>
-        <v>Div2</v>
-      </c>
-      <c r="B81" t="str">
-        <f t="shared" si="27"/>
-        <v>.</v>
-      </c>
-      <c r="C81" s="6">
-        <f t="shared" si="27"/>
-        <v>27.943991726981899</v>
-      </c>
-      <c r="D81" s="6">
-        <f t="shared" si="27"/>
-        <v>0.38424887385039203</v>
-      </c>
-      <c r="E81">
-        <f t="shared" si="27"/>
-        <v>3663</v>
-      </c>
-      <c r="F81" s="6">
-        <f t="shared" si="27"/>
-        <v>26.864738139079702</v>
-      </c>
-      <c r="G81" s="6">
-        <f t="shared" si="27"/>
-        <v>29.0232453148842</v>
-      </c>
-      <c r="H81" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="str">
-        <f t="shared" ref="A82:G82" si="28">A69</f>
-        <v>.</v>
-      </c>
-      <c r="B82" s="4" t="str">
-        <f t="shared" si="28"/>
-        <v>DivNA - Div0</v>
-      </c>
-      <c r="C82" s="5">
-        <f t="shared" si="28"/>
-        <v>-5.3209118691406397E-2</v>
-      </c>
-      <c r="D82" s="5">
-        <f t="shared" si="28"/>
-        <v>0.26259396426173198</v>
-      </c>
-      <c r="E82" s="4">
-        <f t="shared" si="28"/>
-        <v>3663</v>
-      </c>
-      <c r="F82" s="5">
-        <f t="shared" si="28"/>
-        <v>-0.790766200514607</v>
-      </c>
-      <c r="G82" s="5">
-        <f t="shared" si="28"/>
         <v>0.68434796313179402</v>
       </c>
       <c r="H82" s="17">
@@ -3971,217 +3990,210 @@
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="24" t="str">
-        <f t="shared" ref="A83:G83" si="29">A70</f>
+      <c r="A83" t="str">
+        <f t="shared" ref="A83:G83" si="27">A70</f>
         <v>.</v>
       </c>
-      <c r="B83" s="24" t="str">
+      <c r="B83" t="str">
+        <f t="shared" si="27"/>
+        <v>DivNA - Div1</v>
+      </c>
+      <c r="C83" s="6">
+        <f t="shared" si="27"/>
+        <v>0.17986780233115099</v>
+      </c>
+      <c r="D83" s="6">
+        <f t="shared" si="27"/>
+        <v>0.40397849672064401</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="27"/>
+        <v>3663</v>
+      </c>
+      <c r="F83" s="6">
+        <f t="shared" si="27"/>
+        <v>-0.95480108466437197</v>
+      </c>
+      <c r="G83" s="6">
+        <f t="shared" si="27"/>
+        <v>1.3145366893266699</v>
+      </c>
+      <c r="H83" s="16">
+        <f t="shared" ref="H83:H87" si="28">IF(H70&lt;0.0001,"&lt;0.0001",IF(H70&lt;0.001,"&lt;0.001",IF(H70&lt;0.01,"&lt;0.01",ROUND(H70,3))))</f>
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f t="shared" ref="A84:G84" si="29">A71</f>
+        <v>.</v>
+      </c>
+      <c r="B84" t="str">
         <f t="shared" si="29"/>
-        <v>DivNA - Div1</v>
-      </c>
-      <c r="C83" s="30">
+        <v>DivNA - Div2</v>
+      </c>
+      <c r="C84" s="6">
         <f t="shared" si="29"/>
-        <v>0.17986780233115099</v>
-      </c>
-      <c r="D83" s="30">
+        <v>1.31759992374365</v>
+      </c>
+      <c r="D84" s="6">
         <f t="shared" si="29"/>
-        <v>0.40397849672064401</v>
-      </c>
-      <c r="E83" s="24">
+        <v>0.40403740028358298</v>
+      </c>
+      <c r="E84">
         <f t="shared" si="29"/>
         <v>3663</v>
       </c>
-      <c r="F83" s="30">
+      <c r="F84" s="6">
         <f t="shared" si="29"/>
-        <v>-0.95480108466437197</v>
-      </c>
-      <c r="G83" s="30">
+        <v>0.18276559219911501</v>
+      </c>
+      <c r="G84" s="6">
         <f t="shared" si="29"/>
-        <v>1.3145366893266699</v>
-      </c>
-      <c r="H83" s="29">
-        <f t="shared" ref="H83:H87" si="30">IF(H70&lt;0.0001,"&lt;0.0001",IF(H70&lt;0.001,"&lt;0.001",IF(H70&lt;0.01,"&lt;0.01",ROUND(H70,3))))</f>
-        <v>0.97099999999999997</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="str">
-        <f t="shared" ref="A84:G84" si="31">A71</f>
+        <v>2.4524342552881802</v>
+      </c>
+      <c r="H84" s="16" t="str">
+        <f t="shared" si="28"/>
+        <v>&lt;0.01</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f t="shared" ref="A85:G85" si="30">A72</f>
         <v>.</v>
       </c>
-      <c r="B84" s="24" t="str">
+      <c r="B85" t="str">
+        <f t="shared" si="30"/>
+        <v>Div0 - Div1</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" si="30"/>
+        <v>0.233076921022557</v>
+      </c>
+      <c r="D85" s="6">
+        <f t="shared" si="30"/>
+        <v>0.41913953898231698</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="30"/>
+        <v>3663</v>
+      </c>
+      <c r="F85" s="6">
+        <f t="shared" si="30"/>
+        <v>-0.94417532892022604</v>
+      </c>
+      <c r="G85" s="6">
+        <f t="shared" si="30"/>
+        <v>1.4103291709653401</v>
+      </c>
+      <c r="H85" s="16">
+        <f t="shared" si="28"/>
+        <v>0.94499999999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f t="shared" ref="A86:G86" si="31">A73</f>
+        <v>.</v>
+      </c>
+      <c r="B86" t="str">
         <f t="shared" si="31"/>
-        <v>DivNA - Div2</v>
-      </c>
-      <c r="C84" s="30">
+        <v>Div0 - Div2</v>
+      </c>
+      <c r="C86" s="6">
         <f t="shared" si="31"/>
-        <v>1.31759992374365</v>
-      </c>
-      <c r="D84" s="30">
+        <v>1.3708090424350501</v>
+      </c>
+      <c r="D86" s="6">
         <f t="shared" si="31"/>
-        <v>0.40403740028358298</v>
-      </c>
-      <c r="E84" s="24">
+        <v>0.418550383039826</v>
+      </c>
+      <c r="E86">
         <f t="shared" si="31"/>
         <v>3663</v>
       </c>
-      <c r="F84" s="30">
+      <c r="F86" s="6">
         <f t="shared" si="31"/>
-        <v>0.18276559219911501</v>
-      </c>
-      <c r="G84" s="30">
+        <v>0.19521157591009999</v>
+      </c>
+      <c r="G86" s="6">
         <f t="shared" si="31"/>
-        <v>2.4524342552881802</v>
-      </c>
-      <c r="H84" s="29" t="str">
-        <f t="shared" si="30"/>
+        <v>2.5464065089600099</v>
+      </c>
+      <c r="H86" s="16" t="str">
+        <f t="shared" si="28"/>
         <v>&lt;0.01</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="24" t="str">
-        <f t="shared" ref="A85:G85" si="32">A72</f>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="str">
+        <f t="shared" ref="A87:G87" si="32">A74</f>
         <v>.</v>
       </c>
-      <c r="B85" s="24" t="str">
+      <c r="B87" s="3" t="str">
         <f t="shared" si="32"/>
-        <v>Div0 - Div1</v>
-      </c>
-      <c r="C85" s="30">
+        <v>Div1 - Div2</v>
+      </c>
+      <c r="C87" s="7">
         <f t="shared" si="32"/>
-        <v>0.233076921022557</v>
-      </c>
-      <c r="D85" s="30">
+        <v>1.1377321214125</v>
+      </c>
+      <c r="D87" s="7">
         <f t="shared" si="32"/>
-        <v>0.41913953898231698</v>
-      </c>
-      <c r="E85" s="24">
+        <v>0.50975131278956798</v>
+      </c>
+      <c r="E87" s="3">
         <f t="shared" si="32"/>
         <v>3663</v>
       </c>
-      <c r="F85" s="30">
+      <c r="F87" s="7">
         <f t="shared" si="32"/>
-        <v>-0.94417532892022604</v>
-      </c>
-      <c r="G85" s="30">
+        <v>-0.29402466619547102</v>
+      </c>
+      <c r="G87" s="7">
         <f t="shared" si="32"/>
-        <v>1.4103291709653401</v>
-      </c>
-      <c r="H85" s="29">
-        <f t="shared" si="30"/>
-        <v>0.94499999999999995</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="str">
-        <f t="shared" ref="A86:G86" si="33">A73</f>
-        <v>.</v>
-      </c>
-      <c r="B86" s="24" t="str">
-        <f t="shared" si="33"/>
-        <v>Div0 - Div2</v>
-      </c>
-      <c r="C86" s="30">
-        <f t="shared" si="33"/>
-        <v>1.3708090424350501</v>
-      </c>
-      <c r="D86" s="30">
-        <f t="shared" si="33"/>
-        <v>0.418550383039826</v>
-      </c>
-      <c r="E86" s="24">
-        <f t="shared" si="33"/>
-        <v>3663</v>
-      </c>
-      <c r="F86" s="30">
-        <f t="shared" si="33"/>
-        <v>0.19521157591009999</v>
-      </c>
-      <c r="G86" s="30">
-        <f t="shared" si="33"/>
-        <v>2.5464065089600099</v>
-      </c>
-      <c r="H86" s="29" t="str">
-        <f t="shared" si="30"/>
-        <v>&lt;0.01</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="str">
-        <f t="shared" ref="A87:G87" si="34">A74</f>
-        <v>.</v>
-      </c>
-      <c r="B87" s="3" t="str">
-        <f t="shared" si="34"/>
-        <v>Div1 - Div2</v>
-      </c>
-      <c r="C87" s="7">
-        <f t="shared" si="34"/>
-        <v>1.1377321214125</v>
-      </c>
-      <c r="D87" s="7">
-        <f t="shared" si="34"/>
-        <v>0.50975131278956798</v>
-      </c>
-      <c r="E87" s="3">
-        <f t="shared" si="34"/>
-        <v>3663</v>
-      </c>
-      <c r="F87" s="7">
-        <f t="shared" si="34"/>
-        <v>-0.29402466619547102</v>
-      </c>
-      <c r="G87" s="7">
-        <f t="shared" si="34"/>
         <v>2.56948890902046</v>
       </c>
       <c r="H87" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>0.115</v>
       </c>
     </row>
-    <row r="90" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="36" t="s">
+    <row r="90" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="36" t="s">
+    <row r="91" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>50</v>
       </c>
-      <c r="B92"/>
-    </row>
-    <row r="93" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
-      <c r="B93"/>
-    </row>
-    <row r="94" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>49</v>
       </c>
-      <c r="B94"/>
-    </row>
-    <row r="95" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>43</v>
       </c>
-      <c r="K96" s="31" t="s">
+      <c r="K96" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="L96" s="32"/>
-      <c r="M96" s="32"/>
-      <c r="N96" s="32"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="27"/>
+      <c r="N96" s="27"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
@@ -4203,7 +4215,7 @@
       <c r="L97" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M97" s="28" t="s">
+      <c r="M97" s="25" t="s">
         <v>23</v>
       </c>
       <c r="N97" s="1" t="s">
@@ -4223,7 +4235,7 @@
       <c r="E98">
         <v>1427.7153165680099</v>
       </c>
-      <c r="F98" s="23">
+      <c r="F98" s="22">
         <v>6.3199861857458298E-260</v>
       </c>
       <c r="K98" t="str">
@@ -4231,15 +4243,15 @@
         <v>(Intercept)</v>
       </c>
       <c r="L98" s="2">
-        <f t="shared" ref="L98:L106" si="35">C98</f>
+        <f t="shared" ref="L98:L104" si="33">C98</f>
         <v>71155.985807330595</v>
       </c>
       <c r="M98">
-        <f t="shared" ref="M98:M106" si="36">D98</f>
+        <f t="shared" ref="M98:M104" si="34">D98</f>
         <v>1</v>
       </c>
       <c r="N98" s="16" t="str">
-        <f>IF(F98&lt;0.0001,"&lt;0.0001",IF(F98&lt;0.001,"&lt;0.001",IF(F98&lt;0.01,"&lt;0.01",ROUND(F98,3))))</f>
+        <f t="shared" ref="N98:N103" si="35">IF(F98&lt;0.0001,"&lt;0.0001",IF(F98&lt;0.001,"&lt;0.001",IF(F98&lt;0.01,"&lt;0.01",ROUND(F98,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4260,19 +4272,19 @@
         <v>9.9751196472365796E-3</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" ref="K99:K106" si="37">B99</f>
+        <f t="shared" ref="K99:K104" si="36">B99</f>
         <v>DivGroup</v>
       </c>
       <c r="L99" s="2">
+        <f t="shared" si="33"/>
+        <v>566.57462623345805</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="N99" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>566.57462623345805</v>
-      </c>
-      <c r="M99">
-        <f t="shared" si="36"/>
-        <v>3</v>
-      </c>
-      <c r="N99" s="16" t="str">
-        <f>IF(F99&lt;0.0001,"&lt;0.0001",IF(F99&lt;0.001,"&lt;0.001",IF(F99&lt;0.01,"&lt;0.01",ROUND(F99,3))))</f>
         <v>&lt;0.01</v>
       </c>
     </row>
@@ -4293,19 +4305,19 @@
         <v>1.8484315961216299E-6</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>age_3</v>
       </c>
       <c r="L100" s="2">
+        <f t="shared" si="33"/>
+        <v>1321.1492635663899</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="N100" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>1321.1492635663899</v>
-      </c>
-      <c r="M100">
-        <f t="shared" si="36"/>
-        <v>2</v>
-      </c>
-      <c r="N100" s="16" t="str">
-        <f>IF(F100&lt;0.0001,"&lt;0.0001",IF(F100&lt;0.001,"&lt;0.001",IF(F100&lt;0.01,"&lt;0.01",ROUND(F100,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4326,19 +4338,19 @@
         <v>1.36971152716028E-4</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>RIAGENDR</v>
       </c>
       <c r="L101" s="2">
+        <f t="shared" si="33"/>
+        <v>726.53776660599397</v>
+      </c>
+      <c r="M101">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="N101" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>726.53776660599397</v>
-      </c>
-      <c r="M101">
-        <f t="shared" si="36"/>
-        <v>1</v>
-      </c>
-      <c r="N101" s="16" t="str">
-        <f>IF(F101&lt;0.0001,"&lt;0.0001",IF(F101&lt;0.001,"&lt;0.001",IF(F101&lt;0.01,"&lt;0.01",ROUND(F101,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4359,19 +4371,19 @@
         <v>1.17370831488711E-3</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>eth_5</v>
       </c>
       <c r="L102" s="2">
+        <f t="shared" si="33"/>
+        <v>795.58839660667604</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="N102" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>795.58839660667604</v>
-      </c>
-      <c r="M102">
-        <f t="shared" si="36"/>
-        <v>3</v>
-      </c>
-      <c r="N102" s="16" t="str">
-        <f>IF(F102&lt;0.0001,"&lt;0.0001",IF(F102&lt;0.001,"&lt;0.001",IF(F102&lt;0.01,"&lt;0.01",ROUND(F102,3))))</f>
         <v>&lt;0.01</v>
       </c>
     </row>
@@ -4392,52 +4404,52 @@
         <v>0.35841900360058598</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>FIPL</v>
       </c>
       <c r="L103" s="2">
+        <f t="shared" si="33"/>
+        <v>102.30681246263001</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="N103" s="16">
         <f t="shared" si="35"/>
-        <v>102.30681246263001</v>
-      </c>
-      <c r="M103">
+        <v>0.35799999999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" s="2">
+        <v>901.13900327903696</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>9.0404900075586507</v>
+      </c>
+      <c r="F104">
+        <v>1.21475448255204E-4</v>
+      </c>
+      <c r="K104" t="str">
         <f t="shared" si="36"/>
+        <v>edu</v>
+      </c>
+      <c r="L104" s="2">
+        <f t="shared" si="33"/>
+        <v>901.13900327903696</v>
+      </c>
+      <c r="M104">
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
-      <c r="N103" s="16">
-        <f>IF(F103&lt;0.0001,"&lt;0.0001",IF(F103&lt;0.001,"&lt;0.001",IF(F103&lt;0.01,"&lt;0.01",ROUND(F103,3))))</f>
-        <v>0.35799999999999998</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B104" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C104" s="25">
-        <v>901.13900327903696</v>
-      </c>
-      <c r="D104" s="24">
-        <v>2</v>
-      </c>
-      <c r="E104" s="24">
-        <v>9.0404900075586507</v>
-      </c>
-      <c r="F104" s="24">
-        <v>1.21475448255204E-4</v>
-      </c>
-      <c r="K104" t="str">
-        <f t="shared" si="37"/>
-        <v>edu</v>
-      </c>
-      <c r="L104" s="2">
-        <f t="shared" si="35"/>
-        <v>901.13900327903696</v>
-      </c>
-      <c r="M104">
-        <f t="shared" si="36"/>
-        <v>2</v>
-      </c>
       <c r="N104" s="16" t="str">
-        <f t="shared" ref="N104:N105" si="38">IF(F104&lt;0.0001,"&lt;0.0001",IF(F104&lt;0.001,"&lt;0.001",IF(F104&lt;0.01,"&lt;0.01",ROUND(F104,3))))</f>
+        <f t="shared" ref="N104:N105" si="37">IF(F104&lt;0.0001,"&lt;0.0001",IF(F104&lt;0.001,"&lt;0.001",IF(F104&lt;0.01,"&lt;0.01",ROUND(F104,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4458,19 +4470,19 @@
         <v>0.20920720902224901</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" ref="K105:K106" si="39">B105</f>
+        <f t="shared" ref="K105:K106" si="38">B105</f>
         <v>KCAL</v>
       </c>
       <c r="L105" s="2">
-        <f t="shared" ref="L105:L106" si="40">C105</f>
+        <f t="shared" ref="L105:L106" si="39">C105</f>
         <v>78.622123002744004</v>
       </c>
       <c r="M105">
-        <f t="shared" ref="M105:M106" si="41">D105</f>
+        <f t="shared" ref="M105:M106" si="40">D105</f>
         <v>1</v>
       </c>
       <c r="N105" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.20899999999999999</v>
       </c>
     </row>
@@ -4491,24 +4503,17 @@
         <v>27</v>
       </c>
       <c r="K106" t="str">
+        <f t="shared" si="38"/>
+        <v>Residuals</v>
+      </c>
+      <c r="L106" s="2">
         <f t="shared" si="39"/>
-        <v>Residuals</v>
-      </c>
-      <c r="L106" s="2">
+        <v>164369.21175342501</v>
+      </c>
+      <c r="M106">
         <f t="shared" si="40"/>
-        <v>164369.21175342501</v>
-      </c>
-      <c r="M106">
-        <f t="shared" si="41"/>
         <v>3298</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24"/>
-      <c r="F107" s="24"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
@@ -4703,7 +4708,7 @@
       <c r="G114" s="4">
         <v>0.84095323171681302</v>
       </c>
-      <c r="H114" s="26">
+      <c r="H114" s="23">
         <f>O114</f>
         <v>0.99852165952845096</v>
       </c>
@@ -4749,7 +4754,7 @@
       <c r="G115">
         <v>1.3872843328716999</v>
       </c>
-      <c r="H115" s="27">
+      <c r="H115" s="24">
         <f>O115</f>
         <v>0.99737270710040904</v>
       </c>
@@ -4795,8 +4800,8 @@
       <c r="G116" s="8">
         <v>2.8082243038838599</v>
       </c>
-      <c r="H116" s="35">
-        <f t="shared" ref="H116:H119" si="42">O116</f>
+      <c r="H116" s="30">
+        <f t="shared" ref="H116:H119" si="41">O116</f>
         <v>5.6032796572065297E-3</v>
       </c>
       <c r="J116" t="s">
@@ -4841,8 +4846,8 @@
       <c r="G117">
         <v>1.3858939209057901</v>
       </c>
-      <c r="H117" s="27">
-        <f t="shared" si="42"/>
+      <c r="H117" s="24">
+        <f t="shared" si="41"/>
         <v>0.99970939251304503</v>
       </c>
       <c r="J117" t="s">
@@ -4887,8 +4892,8 @@
       <c r="G118" s="8">
         <v>2.8032097586625699</v>
       </c>
-      <c r="H118" s="35">
-        <f t="shared" si="42"/>
+      <c r="H118" s="30">
+        <f t="shared" si="41"/>
         <v>1.07475589106431E-2</v>
       </c>
       <c r="J118" t="s">
@@ -4933,8 +4938,8 @@
       <c r="G119" s="14">
         <v>3.0903349193569198</v>
       </c>
-      <c r="H119" s="34">
-        <f t="shared" si="42"/>
+      <c r="H119" s="29">
+        <f t="shared" si="41"/>
         <v>7.6813834731943795E-2</v>
       </c>
       <c r="J119" t="s">
@@ -4958,16 +4963,16 @@
       <c r="P119" s="13"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A121" s="31" t="s">
+      <c r="A121" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32"/>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="32"/>
-      <c r="H121" s="32"/>
+      <c r="B121" s="27"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="27"/>
+      <c r="H121" s="27"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
@@ -5001,159 +5006,159 @@
         <v>DivNA</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" ref="B123:G123" si="43">B110</f>
+        <f t="shared" ref="B123:G123" si="42">B110</f>
         <v>.</v>
       </c>
       <c r="C123" s="6">
+        <f t="shared" si="42"/>
+        <v>30.1625441474532</v>
+      </c>
+      <c r="D123" s="6">
+        <f t="shared" si="42"/>
+        <v>0.227981112599141</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="42"/>
+        <v>3298</v>
+      </c>
+      <c r="F123" s="6">
+        <f t="shared" si="42"/>
+        <v>29.522162450238699</v>
+      </c>
+      <c r="G123" s="6">
+        <f t="shared" si="42"/>
+        <v>30.802925844667801</v>
+      </c>
+      <c r="H123" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A124" t="str">
+        <f t="shared" ref="A124:G124" si="43">A111</f>
+        <v>Div0</v>
+      </c>
+      <c r="B124" t="str">
         <f t="shared" si="43"/>
-        <v>30.1625441474532</v>
-      </c>
-      <c r="D123" s="6">
+        <v>.</v>
+      </c>
+      <c r="C124" s="6">
         <f t="shared" si="43"/>
-        <v>0.227981112599141</v>
-      </c>
-      <c r="E123">
+        <v>30.1170187444019</v>
+      </c>
+      <c r="D124" s="6">
+        <f t="shared" si="43"/>
+        <v>0.26755203283678303</v>
+      </c>
+      <c r="E124">
         <f t="shared" si="43"/>
         <v>3298</v>
       </c>
-      <c r="F123" s="6">
+      <c r="F124" s="6">
         <f t="shared" si="43"/>
-        <v>29.522162450238699</v>
-      </c>
-      <c r="G123" s="6">
+        <v>29.3654853260065</v>
+      </c>
+      <c r="G124" s="6">
         <f t="shared" si="43"/>
-        <v>30.802925844667801</v>
-      </c>
-      <c r="H123" t="s">
+        <v>30.8685521627973</v>
+      </c>
+      <c r="H124" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A124" t="str">
-        <f t="shared" ref="A124:G124" si="44">A111</f>
-        <v>Div0</v>
-      </c>
-      <c r="B124" t="str">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A125" t="str">
+        <f t="shared" ref="A125:G125" si="44">A112</f>
+        <v>Div1</v>
+      </c>
+      <c r="B125" t="str">
         <f t="shared" si="44"/>
         <v>.</v>
       </c>
-      <c r="C124" s="6">
+      <c r="C125" s="6">
         <f t="shared" si="44"/>
-        <v>30.1170187444019</v>
-      </c>
-      <c r="D124" s="6">
+        <v>30.072476096687598</v>
+      </c>
+      <c r="D125" s="6">
         <f t="shared" si="44"/>
-        <v>0.26755203283678303</v>
-      </c>
-      <c r="E124">
+        <v>0.45053360088992001</v>
+      </c>
+      <c r="E125">
         <f t="shared" si="44"/>
         <v>3298</v>
       </c>
-      <c r="F124" s="6">
+      <c r="F125" s="6">
         <f t="shared" si="44"/>
-        <v>29.3654853260065</v>
-      </c>
-      <c r="G124" s="6">
+        <v>28.806961297234199</v>
+      </c>
+      <c r="G125" s="6">
         <f t="shared" si="44"/>
-        <v>30.8685521627973</v>
-      </c>
-      <c r="H124" t="s">
+        <v>31.3379908961411</v>
+      </c>
+      <c r="H125" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" t="str">
-        <f t="shared" ref="A125:G125" si="45">A112</f>
-        <v>Div1</v>
-      </c>
-      <c r="B125" t="str">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
+        <f t="shared" ref="A126:G126" si="45">A113</f>
+        <v>Div2</v>
+      </c>
+      <c r="B126" t="str">
         <f t="shared" si="45"/>
         <v>.</v>
       </c>
-      <c r="C125" s="6">
+      <c r="C126" s="6">
         <f t="shared" si="45"/>
-        <v>30.072476096687598</v>
-      </c>
-      <c r="D125" s="6">
+        <v>28.6478707556121</v>
+      </c>
+      <c r="D126" s="6">
         <f t="shared" si="45"/>
-        <v>0.45053360088992001</v>
-      </c>
-      <c r="E125">
+        <v>0.45175682989840998</v>
+      </c>
+      <c r="E126">
         <f t="shared" si="45"/>
         <v>3298</v>
       </c>
-      <c r="F125" s="6">
+      <c r="F126" s="6">
         <f t="shared" si="45"/>
-        <v>28.806961297234199</v>
-      </c>
-      <c r="G125" s="6">
+        <v>27.378919998418102</v>
+      </c>
+      <c r="G126" s="6">
         <f t="shared" si="45"/>
-        <v>31.3379908961411</v>
-      </c>
-      <c r="H125" t="s">
+        <v>29.916821512806202</v>
+      </c>
+      <c r="H126" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A126" t="str">
-        <f t="shared" ref="A126:G126" si="46">A113</f>
-        <v>Div2</v>
-      </c>
-      <c r="B126" t="str">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="str">
+        <f t="shared" ref="A127:G127" si="46">A114</f>
+        <v>.</v>
+      </c>
+      <c r="B127" s="4" t="str">
         <f t="shared" si="46"/>
-        <v>.</v>
-      </c>
-      <c r="C126" s="6">
+        <v>DivNA - Div0</v>
+      </c>
+      <c r="C127" s="5">
         <f t="shared" si="46"/>
-        <v>28.6478707556121</v>
-      </c>
-      <c r="D126" s="6">
+        <v>4.5525403051340299E-2</v>
+      </c>
+      <c r="D127" s="5">
         <f t="shared" si="46"/>
-        <v>0.45175682989840998</v>
-      </c>
-      <c r="E126">
+        <v>0.28317880126844203</v>
+      </c>
+      <c r="E127" s="4">
         <f t="shared" si="46"/>
         <v>3298</v>
       </c>
-      <c r="F126" s="6">
+      <c r="F127" s="5">
         <f t="shared" si="46"/>
-        <v>27.378919998418102</v>
-      </c>
-      <c r="G126" s="6">
+        <v>-0.74990242561413201</v>
+      </c>
+      <c r="G127" s="5">
         <f t="shared" si="46"/>
-        <v>29.916821512806202</v>
-      </c>
-      <c r="H126" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="str">
-        <f t="shared" ref="A127:G127" si="47">A114</f>
-        <v>.</v>
-      </c>
-      <c r="B127" s="4" t="str">
-        <f t="shared" si="47"/>
-        <v>DivNA - Div0</v>
-      </c>
-      <c r="C127" s="5">
-        <f t="shared" si="47"/>
-        <v>4.5525403051340299E-2</v>
-      </c>
-      <c r="D127" s="5">
-        <f t="shared" si="47"/>
-        <v>0.28317880126844203</v>
-      </c>
-      <c r="E127" s="4">
-        <f t="shared" si="47"/>
-        <v>3298</v>
-      </c>
-      <c r="F127" s="5">
-        <f t="shared" si="47"/>
-        <v>-0.74990242561413201</v>
-      </c>
-      <c r="G127" s="5">
-        <f t="shared" si="47"/>
         <v>0.84095323171681302</v>
       </c>
       <c r="H127" s="17">
@@ -5162,172 +5167,172 @@
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A128" s="24" t="str">
-        <f t="shared" ref="A128:G128" si="48">A115</f>
+      <c r="A128" t="str">
+        <f t="shared" ref="A128:G128" si="47">A115</f>
         <v>.</v>
       </c>
-      <c r="B128" s="24" t="str">
+      <c r="B128" t="str">
+        <f t="shared" si="47"/>
+        <v>DivNA - Div1</v>
+      </c>
+      <c r="C128" s="6">
+        <f t="shared" si="47"/>
+        <v>9.0068050765607699E-2</v>
+      </c>
+      <c r="D128" s="6">
+        <f t="shared" si="47"/>
+        <v>0.46181958754073099</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="47"/>
+        <v>3298</v>
+      </c>
+      <c r="F128" s="6">
+        <f t="shared" si="47"/>
+        <v>-1.20714823134048</v>
+      </c>
+      <c r="G128" s="6">
+        <f t="shared" si="47"/>
+        <v>1.3872843328716999</v>
+      </c>
+      <c r="H128" s="16">
+        <f t="shared" ref="H128:H132" si="48">IF(H115&lt;0.0001,"&lt;0.0001",IF(H115&lt;0.001,"&lt;0.001",IF(H115&lt;0.01,"&lt;0.01",ROUND(H115,3))))</f>
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f t="shared" ref="A129:G129" si="49">A116</f>
+        <v>.</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="49"/>
+        <v>DivNA - Div2</v>
+      </c>
+      <c r="C129" s="6">
+        <f t="shared" si="49"/>
+        <v>1.5146733918411199</v>
+      </c>
+      <c r="D129" s="6">
+        <f t="shared" si="49"/>
+        <v>0.46051468587229499</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="49"/>
+        <v>3298</v>
+      </c>
+      <c r="F129" s="6">
+        <f t="shared" si="49"/>
+        <v>0.221122479798389</v>
+      </c>
+      <c r="G129" s="6">
+        <f t="shared" si="49"/>
+        <v>2.8082243038838599</v>
+      </c>
+      <c r="H129" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>DivNA - Div1</v>
-      </c>
-      <c r="C128" s="30">
-        <f t="shared" si="48"/>
-        <v>9.0068050765607699E-2</v>
-      </c>
-      <c r="D128" s="30">
-        <f t="shared" si="48"/>
-        <v>0.46181958754073099</v>
-      </c>
-      <c r="E128" s="24">
-        <f t="shared" si="48"/>
-        <v>3298</v>
-      </c>
-      <c r="F128" s="30">
-        <f t="shared" si="48"/>
-        <v>-1.20714823134048</v>
-      </c>
-      <c r="G128" s="30">
-        <f t="shared" si="48"/>
-        <v>1.3872843328716999</v>
-      </c>
-      <c r="H128" s="29">
-        <f t="shared" ref="H128:H132" si="49">IF(H115&lt;0.0001,"&lt;0.0001",IF(H115&lt;0.001,"&lt;0.001",IF(H115&lt;0.01,"&lt;0.01",ROUND(H115,3))))</f>
-        <v>0.997</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="24" t="str">
-        <f t="shared" ref="A129:G129" si="50">A116</f>
+        <v>&lt;0.01</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" t="str">
+        <f t="shared" ref="A130:G130" si="50">A117</f>
         <v>.</v>
       </c>
-      <c r="B129" s="24" t="str">
+      <c r="B130" t="str">
         <f t="shared" si="50"/>
-        <v>DivNA - Div2</v>
-      </c>
-      <c r="C129" s="30">
+        <v>Div0 - Div1</v>
+      </c>
+      <c r="C130" s="6">
         <f t="shared" si="50"/>
-        <v>1.5146733918411199</v>
-      </c>
-      <c r="D129" s="30">
+        <v>4.45426477142674E-2</v>
+      </c>
+      <c r="D130" s="6">
         <f t="shared" si="50"/>
-        <v>0.46051468587229499</v>
-      </c>
-      <c r="E129" s="24">
+        <v>0.477532004706895</v>
+      </c>
+      <c r="E130">
         <f t="shared" si="50"/>
         <v>3298</v>
       </c>
-      <c r="F129" s="30">
+      <c r="F130" s="6">
         <f t="shared" si="50"/>
-        <v>0.221122479798389</v>
-      </c>
-      <c r="G129" s="30">
+        <v>-1.2968086254772599</v>
+      </c>
+      <c r="G130" s="6">
         <f t="shared" si="50"/>
-        <v>2.8082243038838599</v>
-      </c>
-      <c r="H129" s="29" t="str">
-        <f t="shared" si="49"/>
-        <v>&lt;0.01</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="24" t="str">
-        <f t="shared" ref="A130:G130" si="51">A117</f>
+        <v>1.3858939209057901</v>
+      </c>
+      <c r="H130" s="16">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" t="str">
+        <f t="shared" ref="A131:G131" si="51">A118</f>
         <v>.</v>
       </c>
-      <c r="B130" s="24" t="str">
+      <c r="B131" t="str">
         <f t="shared" si="51"/>
-        <v>Div0 - Div1</v>
-      </c>
-      <c r="C130" s="30">
+        <v>Div0 - Div2</v>
+      </c>
+      <c r="C131" s="6">
         <f t="shared" si="51"/>
-        <v>4.45426477142674E-2</v>
-      </c>
-      <c r="D130" s="30">
+        <v>1.46914798878978</v>
+      </c>
+      <c r="D131" s="6">
         <f t="shared" si="51"/>
-        <v>0.477532004706895</v>
-      </c>
-      <c r="E130" s="24">
+        <v>0.47493688201033801</v>
+      </c>
+      <c r="E131">
         <f t="shared" si="51"/>
         <v>3298</v>
       </c>
-      <c r="F130" s="30">
+      <c r="F131" s="6">
         <f t="shared" si="51"/>
-        <v>-1.2968086254772599</v>
-      </c>
-      <c r="G130" s="30">
+        <v>0.13508621891699499</v>
+      </c>
+      <c r="G131" s="6">
         <f t="shared" si="51"/>
-        <v>1.3858939209057901</v>
-      </c>
-      <c r="H130" s="29">
-        <f t="shared" si="49"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="24" t="str">
-        <f t="shared" ref="A131:G131" si="52">A118</f>
+        <v>2.8032097586625699</v>
+      </c>
+      <c r="H131" s="16">
+        <f t="shared" si="48"/>
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="str">
+        <f t="shared" ref="A132:G132" si="52">A119</f>
         <v>.</v>
       </c>
-      <c r="B131" s="24" t="str">
+      <c r="B132" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>Div0 - Div2</v>
-      </c>
-      <c r="C131" s="30">
+        <v>Div1 - Div2</v>
+      </c>
+      <c r="C132" s="7">
         <f t="shared" si="52"/>
-        <v>1.46914798878978</v>
-      </c>
-      <c r="D131" s="30">
+        <v>1.42460534107551</v>
+      </c>
+      <c r="D132" s="7">
         <f t="shared" si="52"/>
-        <v>0.47493688201033801</v>
-      </c>
-      <c r="E131" s="24">
+        <v>0.59301332970272203</v>
+      </c>
+      <c r="E132" s="3">
         <f t="shared" si="52"/>
         <v>3298</v>
       </c>
-      <c r="F131" s="30">
+      <c r="F132" s="7">
         <f t="shared" si="52"/>
-        <v>0.13508621891699499</v>
-      </c>
-      <c r="G131" s="30">
+        <v>-0.24112423720589601</v>
+      </c>
+      <c r="G132" s="7">
         <f t="shared" si="52"/>
-        <v>2.8032097586625699</v>
-      </c>
-      <c r="H131" s="29">
-        <f t="shared" si="49"/>
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="str">
-        <f t="shared" ref="A132:G132" si="53">A119</f>
-        <v>.</v>
-      </c>
-      <c r="B132" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>Div1 - Div2</v>
-      </c>
-      <c r="C132" s="7">
-        <f t="shared" si="53"/>
-        <v>1.42460534107551</v>
-      </c>
-      <c r="D132" s="7">
-        <f t="shared" si="53"/>
-        <v>0.59301332970272203</v>
-      </c>
-      <c r="E132" s="3">
-        <f t="shared" si="53"/>
-        <v>3298</v>
-      </c>
-      <c r="F132" s="7">
-        <f t="shared" si="53"/>
-        <v>-0.24112423720589601</v>
-      </c>
-      <c r="G132" s="7">
-        <f t="shared" si="53"/>
         <v>3.0903349193569198</v>
       </c>
       <c r="H132" s="18">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>7.6999999999999999E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add factor() to VVKAJ ordination
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
+++ b/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\BMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E122B2F2-D2ED-4556-B77B-821765492615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79DB6D-A411-4CA5-90D1-21E8BA2B7F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="-3045" windowWidth="16620" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW(6.28)" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="60">
   <si>
     <t>Plain means</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Family IPR</t>
   </si>
 </sst>
 </file>
@@ -2949,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF98E2F-A81A-48C0-B8A9-C127F15DCEAA}">
   <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2961,8 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3081,14 +3085,19 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>24</v>
+      <c r="O13" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -3111,16 +3120,23 @@
         <f>B14</f>
         <v>(Intercept)</v>
       </c>
-      <c r="L14" s="2">
-        <f t="shared" ref="L14:M22" si="0">C14</f>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2">
+        <f>C14</f>
         <v>75713.259375285095</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
+      <c r="N14">
+        <f>D14</f>
         <v>1</v>
       </c>
-      <c r="N14" s="16" t="str">
-        <f t="shared" ref="N14:N21" si="1">IF(F14&lt;0.0001,"&lt;0.0001",IF(F14&lt;0.001,"&lt;0.001",IF(F14&lt;0.01,"&lt;0.01",ROUND(F14,3))))</f>
+      <c r="O14" s="2">
+        <f>E14</f>
+        <v>1619.6592675914901</v>
+      </c>
+      <c r="P14" s="16" t="str">
+        <f>IF(F14&lt;0.0001,"&lt;0.0001",IF(F14&lt;0.001,"&lt;0.001",IF(F14&lt;0.01,"&lt;0.01",ROUND(F14,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S14" s="1" t="s">
@@ -3147,26 +3163,32 @@
         <v>6.4274207378343497E-3</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" ref="K15:K22" si="2">B15</f>
+        <f t="shared" ref="K15:K22" si="0">B15</f>
         <v>DivGroup</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
+      <c r="L15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" ref="M15:M21" si="1">C15</f>
         <v>575.80939400632599</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
+      <c r="N15">
+        <f>D15</f>
         <v>3</v>
       </c>
-      <c r="N15" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O15" s="2">
+        <f>E15</f>
+        <v>4.1059079526433102</v>
+      </c>
+      <c r="P15" s="16" t="str">
+        <f>IF(F15&lt;0.0001,"&lt;0.0001",IF(F15&lt;0.001,"&lt;0.001",IF(F15&lt;0.01,"&lt;0.01",ROUND(F15,3))))</f>
         <v>&lt;0.01</v>
       </c>
       <c r="S15" t="s">
         <v>2</v>
       </c>
       <c r="T15" s="2">
-        <f>C39</f>
         <v>29.233804878220202</v>
       </c>
     </row>
@@ -3187,26 +3209,32 @@
         <v>5.59426293768993E-6</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>age_3</v>
       </c>
-      <c r="L16" s="2">
-        <f t="shared" si="0"/>
+      <c r="L16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
         <v>1134.4612065107201</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
+      <c r="N16">
+        <f>D16</f>
         <v>2</v>
       </c>
-      <c r="N16" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O16" s="2">
+        <f>E16</f>
+        <v>12.134206227607599</v>
+      </c>
+      <c r="P16" s="16" t="str">
+        <f>IF(F16&lt;0.0001,"&lt;0.0001",IF(F16&lt;0.001,"&lt;0.001",IF(F16&lt;0.01,"&lt;0.01",ROUND(F16,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S16" t="s">
         <v>3</v>
       </c>
       <c r="T16" s="2">
-        <f t="shared" ref="T16:T18" si="3">C40</f>
         <v>29.241590661609401</v>
       </c>
     </row>
@@ -3227,26 +3255,32 @@
         <v>2.4300614627646399E-4</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>RIAGENDR</v>
       </c>
-      <c r="L17" s="2">
-        <f t="shared" si="0"/>
+      <c r="L17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
         <v>630.71578841036501</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
+      <c r="N17">
+        <f>D17</f>
         <v>1</v>
       </c>
-      <c r="N17" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O17" s="2">
+        <f>E17</f>
+        <v>13.492282333952501</v>
+      </c>
+      <c r="P17" s="16" t="str">
+        <f>IF(F17&lt;0.0001,"&lt;0.0001",IF(F17&lt;0.001,"&lt;0.001",IF(F17&lt;0.01,"&lt;0.01",ROUND(F17,3))))</f>
         <v>&lt;0.001</v>
       </c>
       <c r="S17" t="s">
         <v>4</v>
       </c>
       <c r="T17" s="2">
-        <f t="shared" si="3"/>
         <v>29.038371512135399</v>
       </c>
     </row>
@@ -3267,26 +3301,32 @@
         <v>2.72818096336386E-26</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>eth_5</v>
       </c>
-      <c r="L18" s="2">
-        <f t="shared" si="0"/>
+      <c r="L18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
         <v>5994.1405933300603</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="0"/>
+      <c r="N18">
+        <f>D18</f>
         <v>4</v>
       </c>
-      <c r="N18" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O18" s="2">
+        <f>E18</f>
+        <v>32.0566880997415</v>
+      </c>
+      <c r="P18" s="16" t="str">
+        <f>IF(F18&lt;0.0001,"&lt;0.0001",IF(F18&lt;0.001,"&lt;0.001",IF(F18&lt;0.01,"&lt;0.01",ROUND(F18,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S18" t="s">
         <v>5</v>
       </c>
       <c r="T18" s="2">
-        <f t="shared" si="3"/>
         <v>27.846636199183202</v>
       </c>
     </row>
@@ -3307,19 +3347,26 @@
         <v>0.46195124542618099</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>FIPL</v>
       </c>
-      <c r="L19" s="2">
-        <f t="shared" si="0"/>
+      <c r="L19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
         <v>72.219511814502795</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="0"/>
+      <c r="N19">
+        <f>D19</f>
         <v>2</v>
       </c>
-      <c r="N19" s="16">
-        <f t="shared" si="1"/>
+      <c r="O19" s="2">
+        <f>E19</f>
+        <v>0.77246048166746295</v>
+      </c>
+      <c r="P19" s="16">
+        <f>IF(F19&lt;0.0001,"&lt;0.0001",IF(F19&lt;0.001,"&lt;0.001",IF(F19&lt;0.01,"&lt;0.01",ROUND(F19,3))))</f>
         <v>0.46200000000000002</v>
       </c>
     </row>
@@ -3340,19 +3387,26 @@
         <v>3.9835111970400102E-4</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>edu</v>
       </c>
-      <c r="L20" s="2">
-        <f t="shared" si="0"/>
+      <c r="L20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
         <v>733.461115876853</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="0"/>
+      <c r="N20">
+        <f>D20</f>
         <v>2</v>
       </c>
-      <c r="N20" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O20" s="2">
+        <f>E20</f>
+        <v>7.8451060194069697</v>
+      </c>
+      <c r="P20" s="16" t="str">
+        <f>IF(F20&lt;0.0001,"&lt;0.0001",IF(F20&lt;0.001,"&lt;0.001",IF(F20&lt;0.01,"&lt;0.01",ROUND(F20,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -3373,19 +3427,26 @@
         <v>0.20186199649700501</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>KCAL</v>
       </c>
-      <c r="L21" s="2">
-        <f t="shared" si="0"/>
+      <c r="L21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
         <v>76.170573350013001</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
+      <c r="N21">
+        <f>D21</f>
         <v>1</v>
       </c>
-      <c r="N21" s="16">
-        <f t="shared" si="1"/>
+      <c r="O21" s="2">
+        <f>E21</f>
+        <v>1.6294421355261</v>
+      </c>
+      <c r="P21" s="16">
+        <f>IF(F21&lt;0.0001,"&lt;0.0001",IF(F21&lt;0.001,"&lt;0.001",IF(F21&lt;0.01,"&lt;0.01",ROUND(F21,3))))</f>
         <v>0.20200000000000001</v>
       </c>
     </row>
@@ -3405,18 +3466,23 @@
       <c r="F22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K22" t="str">
-        <f t="shared" si="2"/>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>Residuals</v>
       </c>
-      <c r="L22" s="2">
-        <f t="shared" si="0"/>
+      <c r="L22" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="32">
+        <f>C22</f>
         <v>169455.74339443899</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="0"/>
+      <c r="N22" s="1">
+        <f>D22</f>
         <v>3625</v>
       </c>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -3704,7 +3770,7 @@
         <v>2.5448812352880101</v>
       </c>
       <c r="H32" s="30">
-        <f t="shared" ref="H32:H35" si="4">O32</f>
+        <f t="shared" ref="H32:H35" si="2">O32</f>
         <v>4.2946280616171801E-3</v>
       </c>
       <c r="J32" t="s">
@@ -3750,7 +3816,7 @@
         <v>1.3801541831400499</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.96245091685531103</v>
       </c>
       <c r="J33" t="s">
@@ -3796,7 +3862,7 @@
         <v>2.5856835278199002</v>
       </c>
       <c r="H34" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5.57150409061125E-3</v>
       </c>
       <c r="J34" t="s">
@@ -3842,7 +3908,7 @@
         <v>2.6285234816091898</v>
       </c>
       <c r="H35" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.1538905871083404E-2</v>
       </c>
       <c r="J35" t="s">
@@ -3909,27 +3975,27 @@
         <v>DivNA</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" ref="B39:G39" si="5">B26</f>
+        <f t="shared" ref="B39:G39" si="3">B26</f>
         <v>.</v>
       </c>
       <c r="C39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.233804878220202</v>
       </c>
       <c r="D39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.20968120301689799</v>
       </c>
       <c r="E39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3625</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>28.644862022538302</v>
       </c>
       <c r="G39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.822747733902101</v>
       </c>
       <c r="H39" t="s">
@@ -3938,31 +4004,31 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" ref="A40:G48" si="6">A27</f>
+        <f t="shared" ref="A40:G48" si="4">A27</f>
         <v>Div0</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.241590661609401</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.24374289869233201</v>
       </c>
       <c r="E40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.556976892026601</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.9262044311922</v>
       </c>
       <c r="H40" t="s">
@@ -3971,31 +4037,31 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div1</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.038371512135399</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.38453660956396801</v>
       </c>
       <c r="E41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>27.9583028856091</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>30.1184401386618</v>
       </c>
       <c r="H41" t="s">
@@ -4004,31 +4070,31 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div2</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>27.846636199183202</v>
       </c>
       <c r="D42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.39079291078135497</v>
       </c>
       <c r="E42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>26.748995163437701</v>
       </c>
       <c r="G42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.944277234928698</v>
       </c>
       <c r="H42" t="s">
@@ -4037,31 +4103,31 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B43" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div0</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-7.78578338916802E-3</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.26435514357971601</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.75029427215198097</v>
       </c>
       <c r="G43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.73472270537364504</v>
       </c>
       <c r="H43" s="17">
@@ -4071,171 +4137,171 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div1</v>
       </c>
       <c r="C44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.19543336608478501</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.40463655535146398</v>
       </c>
       <c r="E44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.941091057627087</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3319577897966599</v>
       </c>
       <c r="H44" s="16">
-        <f t="shared" ref="H44:H48" si="7">IF(H31&lt;0.0001,"&lt;0.0001",IF(H31&lt;0.001,"&lt;0.001",IF(H31&lt;0.01,"&lt;0.01",ROUND(H31,3))))</f>
+        <f t="shared" ref="H44:H48" si="5">IF(H31&lt;0.0001,"&lt;0.0001",IF(H31&lt;0.001,"&lt;0.001",IF(H31&lt;0.01,"&lt;0.01",ROUND(H31,3))))</f>
         <v>0.96299999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div2</v>
       </c>
       <c r="C45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3871686790370099</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.41218016179412997</v>
       </c>
       <c r="E45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.22945612278602101</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.5448812352880101</v>
       </c>
       <c r="H45" s="16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>&lt;0.01</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div0 - Div1</v>
       </c>
       <c r="C46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.203219149473953</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.419023936449816</v>
       </c>
       <c r="E46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.97371588419213895</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3801541831400499</v>
       </c>
       <c r="H46" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div0 - Div2</v>
       </c>
       <c r="C47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.39495446242618</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.423935022710899</v>
       </c>
       <c r="E47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.20422539703246001</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.5856835278199002</v>
       </c>
       <c r="H47" s="16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>&lt;0.01</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div1 - Div2</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.1917353129522299</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.51153939431967799</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.24505285570473401</v>
       </c>
       <c r="G48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.6285234816091898</v>
       </c>
       <c r="H48" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -4305,26 +4371,26 @@
         <v>0</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ref="J55:J61" si="8">B55</f>
+        <f t="shared" ref="J55:J61" si="6">B55</f>
         <v>(Intercept)</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" ref="L55:M61" si="9">C55</f>
+        <f t="shared" ref="L55:M61" si="7">C55</f>
         <v>161079.753365293</v>
       </c>
       <c r="M55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N55" s="2">
-        <f>E55</f>
+        <f t="shared" ref="N55:N60" si="8">E55</f>
         <v>3445.7599769502699</v>
       </c>
       <c r="O55" s="16" t="str">
-        <f>IF(F55&lt;0.0001,"&lt;0.0001",IF(F55&lt;0.001,"&lt;0.001",IF(F55&lt;0.01,"&lt;0.01",ROUND(F55,3))))</f>
+        <f t="shared" ref="O55:O60" si="9">IF(F55&lt;0.0001,"&lt;0.0001",IF(F55&lt;0.001,"&lt;0.001",IF(F55&lt;0.01,"&lt;0.01",ROUND(F55,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4345,26 +4411,26 @@
         <v>8.2062289630025296E-3</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>DivGroup</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L56" s="2">
+        <f t="shared" si="7"/>
+        <v>551.12872435804502</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="8"/>
+        <v>3.92984895342282</v>
+      </c>
+      <c r="O56" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>551.12872435804502</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="N56" s="2">
-        <f>E56</f>
-        <v>3.92984895342282</v>
-      </c>
-      <c r="O56" s="16" t="str">
-        <f>IF(F56&lt;0.0001,"&lt;0.0001",IF(F56&lt;0.001,"&lt;0.001",IF(F56&lt;0.01,"&lt;0.01",ROUND(F56,3))))</f>
         <v>&lt;0.01</v>
       </c>
     </row>
@@ -4385,26 +4451,26 @@
         <v>9.2947095523864707E-6</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>age_3</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>51</v>
       </c>
       <c r="L57" s="2">
+        <f t="shared" si="7"/>
+        <v>1086.69973258706</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="8"/>
+        <v>11.623144334655599</v>
+      </c>
+      <c r="O57" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>1086.69973258706</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="N57" s="2">
-        <f>E57</f>
-        <v>11.623144334655599</v>
-      </c>
-      <c r="O57" s="16" t="str">
-        <f>IF(F57&lt;0.0001,"&lt;0.0001",IF(F57&lt;0.001,"&lt;0.001",IF(F57&lt;0.01,"&lt;0.01",ROUND(F57,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4425,26 +4491,26 @@
         <v>5.3179708572879795E-4</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>RIAGENDR</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>52</v>
       </c>
       <c r="L58" s="2">
+        <f t="shared" si="7"/>
+        <v>562.00738546336697</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="8"/>
+        <v>12.0222592543241</v>
+      </c>
+      <c r="O58" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>562.00738546336697</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="N58" s="2">
-        <f>E58</f>
-        <v>12.0222592543241</v>
-      </c>
-      <c r="O58" s="16" t="str">
-        <f>IF(F58&lt;0.0001,"&lt;0.0001",IF(F58&lt;0.001,"&lt;0.001",IF(F58&lt;0.01,"&lt;0.01",ROUND(F58,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4465,26 +4531,26 @@
         <v>1.6934425061199598E-27</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>eth_5</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>53</v>
       </c>
       <c r="L59" s="2">
+        <f t="shared" si="7"/>
+        <v>6267.5231195289198</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="8"/>
+        <v>33.518148415132501</v>
+      </c>
+      <c r="O59" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>6267.5231195289198</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="N59" s="2">
-        <f>E59</f>
-        <v>33.518148415132501</v>
-      </c>
-      <c r="O59" s="16" t="str">
-        <f>IF(F59&lt;0.0001,"&lt;0.0001",IF(F59&lt;0.001,"&lt;0.001",IF(F59&lt;0.01,"&lt;0.01",ROUND(F59,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4505,26 +4571,26 @@
         <v>1.22230982793797E-4</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>edu</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>54</v>
       </c>
       <c r="L60" s="2">
+        <f t="shared" si="7"/>
+        <v>844.44291276141303</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N60" s="2">
+        <f t="shared" si="8"/>
+        <v>9.03200908500874</v>
+      </c>
+      <c r="O60" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>844.44291276141303</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="N60" s="2">
-        <f>E60</f>
-        <v>9.03200908500874</v>
-      </c>
-      <c r="O60" s="16" t="str">
-        <f>IF(F60&lt;0.0001,"&lt;0.0001",IF(F60&lt;0.001,"&lt;0.001",IF(F60&lt;0.01,"&lt;0.01",ROUND(F60,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4545,18 +4611,18 @@
         <v>27</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>Residuals</v>
       </c>
       <c r="K61" s="32" t="s">
         <v>26</v>
       </c>
       <c r="L61" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>169598.97065335201</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3628</v>
       </c>
       <c r="N61" s="33"/>

</xml_diff>